<commit_message>
Slight edit to Excel
</commit_message>
<xml_diff>
--- a/prijateli_tree/app/languages/language_6person 12242023.xlsx
+++ b/prijateli_tree/app/languages/language_6person 12242023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pepi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fdmol\Desktop\Prijateli-project\PrijateliTree\prijateli_tree\app\languages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E86227EE-2657-4D62-A050-4C777DF051F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01D5F6B-1E89-45A8-ABB7-3087E8504554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{32563650-FBFB-490E-A358-48AFEBEBCE91}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{32563650-FBFB-490E-A358-48AFEBEBCE91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -854,9 +854,6 @@
     <t>Kompjutori të paraqet:</t>
   </si>
   <si>
-    <t>Topi yt</t>
-  </si>
-  <si>
     <t>I presim të tjerët...</t>
   </si>
   <si>
@@ -933,6 +930,9 @@
   </si>
   <si>
     <t>Në vend që t'ju caktojmë në mënyrë të rastësishme bashkëmoshatarët që vëzhgoni, ne do t'ju lejojmë të zgjidhni lojtarët që vëzhgoni.</t>
+  </si>
+  <si>
+    <t>Topi yt:</t>
   </si>
 </sst>
 </file>
@@ -1370,23 +1370,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CDA7EC-5237-4A8D-9F9A-44859C7C28D4}">
   <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="3"/>
-    <col min="2" max="2" width="50.59765625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="47.86328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="38.265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.86328125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="32.86328125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="2" max="2" width="50.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="47.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="38.21875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="32.88671875" style="7" customWidth="1"/>
     <col min="7" max="7" width="44" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="3"/>
+    <col min="8" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -1525,8 +1525,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="8" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>0</v>
       </c>
@@ -1618,8 +1618,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="13" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>2</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>3</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>3</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>3</v>
       </c>
@@ -1820,13 +1820,13 @@
         <v>235</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>265</v>
+        <v>291</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>3</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>4</v>
       </c>
@@ -1866,13 +1866,13 @@
         <v>94</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>5</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>5</v>
       </c>
@@ -1912,13 +1912,13 @@
         <v>236</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>6</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>6</v>
       </c>
@@ -1958,13 +1958,13 @@
         <v>237</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>6</v>
       </c>
@@ -1981,13 +1981,13 @@
         <v>238</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>6</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>7</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>7</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>7</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>7</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>8</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>8</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>8</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>8</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>9</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>9</v>
       </c>
@@ -2240,8 +2240,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="41" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>0</v>
       </c>
@@ -2258,13 +2258,13 @@
         <v>239</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>0</v>
       </c>
@@ -2281,13 +2281,13 @@
         <v>240</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>0</v>
       </c>
@@ -2304,13 +2304,13 @@
         <v>241</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>0</v>
       </c>
@@ -2327,13 +2327,13 @@
         <v>242</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>0</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>0</v>
       </c>
@@ -2373,13 +2373,13 @@
         <v>244</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>0</v>
       </c>
@@ -2396,13 +2396,13 @@
         <v>245</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>0</v>
       </c>
@@ -2419,13 +2419,13 @@
         <v>246</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>0</v>
       </c>
@@ -2442,13 +2442,13 @@
         <v>247</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>0</v>
       </c>
@@ -2465,13 +2465,13 @@
         <v>248</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>0</v>
       </c>
@@ -2488,13 +2488,13 @@
         <v>249</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>0</v>
       </c>
@@ -2511,13 +2511,13 @@
         <v>250</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>0</v>
       </c>
@@ -2534,13 +2534,13 @@
         <v>251</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>0</v>
       </c>
@@ -2557,13 +2557,13 @@
         <v>252</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>0</v>
       </c>
@@ -2580,13 +2580,13 @@
         <v>253</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>0</v>
       </c>
@@ -2603,13 +2603,13 @@
         <v>254</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>0</v>
       </c>
@@ -2626,13 +2626,13 @@
         <v>255</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>0</v>
       </c>
@@ -2649,13 +2649,13 @@
         <v>256</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>0</v>
       </c>
@@ -2672,13 +2672,13 @@
         <v>257</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>0</v>
       </c>
@@ -2695,13 +2695,13 @@
         <v>258</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>0</v>
       </c>
@@ -2718,16 +2718,16 @@
         <v>259</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>10</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>10</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>10</v>
       </c>
@@ -2790,13 +2790,13 @@
         <v>226</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>10</v>
       </c>
@@ -2813,37 +2813,37 @@
         <v>230</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="68" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="69" spans="1:7" ht="128.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="70" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="71" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="72" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="73" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="74" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="75" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="76" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="77" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="78" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="79" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="80" spans="1:7" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="81" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="82" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="83" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="84" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="85" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="86" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="87" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="88" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="89" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="90" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="91" ht="14.25" x14ac:dyDescent="0.45"/>
+    <row r="67" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:7" ht="128.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="85" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="90" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2858,16 +2858,16 @@
       <selection activeCell="A2" sqref="A2:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="22.1328125" customWidth="1"/>
-    <col min="3" max="3" width="33.265625" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="33.21875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="18.265625" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Template, excel and en json edit
</commit_message>
<xml_diff>
--- a/prijateli_tree/app/languages/language_6person 12242023.xlsx
+++ b/prijateli_tree/app/languages/language_6person 12242023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fdmol\Desktop\Prijateli-project\PrijateliTree\prijateli_tree\app\languages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01D5F6B-1E89-45A8-ABB7-3087E8504554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE4BA18-C733-4CA2-ADB5-8A7CE8C2D835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{32563650-FBFB-490E-A358-48AFEBEBCE91}"/>
   </bookViews>
@@ -521,9 +521,6 @@
     <t>you_guessed_correctly</t>
   </si>
   <si>
-    <t>You guessed correctly in {X} games, and earned {Y} points, which means you made extra.</t>
-  </si>
-  <si>
     <t>Погодивте правилно во {X} игри и добивте {x} поени, што значи дека сте стекнале дополнителни</t>
   </si>
   <si>
@@ -933,6 +930,9 @@
   </si>
   <si>
     <t>Topi yt:</t>
+  </si>
+  <si>
+    <t>You guessed correctly in {X} games, and earned {x} points, which means you made extra.</t>
   </si>
 </sst>
 </file>
@@ -1370,8 +1370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CDA7EC-5237-4A8D-9F9A-44859C7C28D4}">
   <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1540,10 +1540,10 @@
         <v>34</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>35</v>
@@ -1633,10 +1633,10 @@
         <v>52</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>35</v>
@@ -1656,10 +1656,10 @@
         <v>54</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>35</v>
@@ -1794,10 +1794,10 @@
         <v>83</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>35</v>
@@ -1817,10 +1817,10 @@
         <v>85</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>35</v>
@@ -1866,7 +1866,7 @@
         <v>94</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>95</v>
@@ -1909,10 +1909,10 @@
         <v>102</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>35</v>
@@ -1955,10 +1955,10 @@
         <v>109</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>35</v>
@@ -1978,10 +1978,10 @@
         <v>111</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>35</v>
@@ -2182,16 +2182,16 @@
         <v>153</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E37" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="F37" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="G37" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -2199,22 +2199,22 @@
         <v>9</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="F38" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="G38" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -2222,22 +2222,22 @@
         <v>9</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="E39" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="G39" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>
@@ -2246,19 +2246,19 @@
         <v>0</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="E41" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>35</v>
@@ -2269,19 +2269,19 @@
         <v>0</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C42" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="E42" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>35</v>
@@ -2292,19 +2292,19 @@
         <v>0</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>175</v>
-      </c>
       <c r="E43" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>35</v>
@@ -2315,19 +2315,19 @@
         <v>0</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="E44" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>35</v>
@@ -2338,19 +2338,19 @@
         <v>0</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="E45" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>35</v>
@@ -2361,19 +2361,19 @@
         <v>0</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="E46" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>35</v>
@@ -2384,19 +2384,19 @@
         <v>0</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="E47" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>35</v>
@@ -2407,19 +2407,19 @@
         <v>0</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="E48" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>35</v>
@@ -2430,19 +2430,19 @@
         <v>0</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="E49" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>35</v>
@@ -2453,19 +2453,19 @@
         <v>0</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="E50" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>35</v>
@@ -2476,19 +2476,19 @@
         <v>0</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="E51" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>35</v>
@@ -2499,19 +2499,19 @@
         <v>0</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C52" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="E52" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>35</v>
@@ -2522,19 +2522,19 @@
         <v>0</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="E53" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>35</v>
@@ -2545,19 +2545,19 @@
         <v>0</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="E54" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>35</v>
@@ -2568,19 +2568,19 @@
         <v>0</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="E55" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>35</v>
@@ -2591,19 +2591,19 @@
         <v>0</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C56" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="E56" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>35</v>
@@ -2614,19 +2614,19 @@
         <v>0</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C57" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="E57" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>35</v>
@@ -2637,19 +2637,19 @@
         <v>0</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C58" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="E58" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>35</v>
@@ -2660,19 +2660,19 @@
         <v>0</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="E59" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>35</v>
@@ -2683,19 +2683,19 @@
         <v>0</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C60" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="E60" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>35</v>
@@ -2706,19 +2706,19 @@
         <v>0</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C61" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>211</v>
-      </c>
       <c r="E61" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>35</v>
@@ -2732,22 +2732,22 @@
         <v>10</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="D63" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="E63" s="9" t="s">
+      <c r="F63" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="F63" s="9" t="s">
+      <c r="G63" s="6" t="s">
         <v>216</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2755,22 +2755,22 @@
         <v>10</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C64" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="E64" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="E64" s="9" t="s">
+      <c r="F64" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="F64" s="9" t="s">
+      <c r="G64" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2778,22 +2778,22 @@
         <v>10</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="D65" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="E65" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="E65" s="9" t="s">
+      <c r="F65" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
@@ -2801,22 +2801,22 @@
         <v>10</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C66" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="E66" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E66" s="9" t="s">
+      <c r="F66" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>